<commit_message>
filters may be customFilters or just filters
</commit_message>
<xml_diff>
--- a/spec/integration/data/test-issue-1669.xlsx
+++ b/spec/integration/data/test-issue-1669.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BE85F1-FBEB-41F7-913B-6E80D1819AA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6589642F-F82A-472B-82D1-C9CF764DAEF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-495" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>a</t>
   </si>
@@ -41,16 +42,58 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>T123456789</t>
+  </si>
+  <si>
+    <t>T123456790</t>
+  </si>
+  <si>
+    <t>T123456791</t>
+  </si>
+  <si>
+    <t>T123456792</t>
+  </si>
+  <si>
+    <t>T123456793</t>
+  </si>
+  <si>
+    <t>Test 89</t>
+  </si>
+  <si>
+    <t>Test 90</t>
+  </si>
+  <si>
+    <t>Test 91</t>
+  </si>
+  <si>
+    <t>Test 92</t>
+  </si>
+  <si>
+    <t>Test 93</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,6 +152,25 @@
     <tableColumn id="2" xr3:uid="{4D5A15A7-C106-47A2-86F1-3B6E3741CF76}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F8AC402-4E69-4B5E-A3C9-2E2B0CED770E}" name="Table2" displayName="Table2" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{5DF240FE-61A3-49AC-8B6E-73051C9D8F0C}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="T123456789"/>
+        <filter val="T123456791"/>
+        <filter val="T123456793"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{ED927DB7-B7DA-4D43-80D8-1468E2B64B5C}" name="DK"/>
+    <tableColumn id="2" xr3:uid="{BAE49BA7-67BA-4374-A131-7971F8F8DE7F}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -377,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -440,4 +502,74 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F35607C-A4E3-4557-9EE1-5DCE8928D2D3}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>